<commit_message>
[UPD] add webserver.py for Task 4       python_exercise.py add function for write excel file       README.md add information on file.py
</commit_message>
<xml_diff>
--- a/Report_excel.xlsx
+++ b/Report_excel.xlsx
@@ -31,46 +31,46 @@
     <t>Campania</t>
   </si>
   <si>
+    <t>Lazio</t>
+  </si>
+  <si>
     <t>Emilia-Romagna</t>
   </si>
   <si>
-    <t>Lazio</t>
+    <t>Sicilia</t>
   </si>
   <si>
     <t>Piemonte</t>
   </si>
   <si>
+    <t>Puglia</t>
+  </si>
+  <si>
     <t>Toscana</t>
   </si>
   <si>
-    <t>Sicilia</t>
-  </si>
-  <si>
-    <t>Puglia</t>
+    <t>Marche</t>
   </si>
   <si>
     <t>Liguria</t>
   </si>
   <si>
-    <t>Marche</t>
+    <t>Abruzzo</t>
+  </si>
+  <si>
+    <t>Calabria</t>
   </si>
   <si>
     <t>Friuli Venezia Giulia</t>
   </si>
   <si>
-    <t>Abruzzo</t>
-  </si>
-  <si>
-    <t>Calabria</t>
+    <t>Sardegna</t>
+  </si>
+  <si>
+    <t>Umbria</t>
   </si>
   <si>
     <t>P.A. Bolzano</t>
-  </si>
-  <si>
-    <t>Umbria</t>
-  </si>
-  <si>
-    <t>Sardegna</t>
   </si>
   <si>
     <t>P.A. Trento</t>
@@ -462,7 +462,7 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>2338306</v>
+        <v>4140912</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -473,7 +473,7 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>1334054</v>
+        <v>2710818</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -484,7 +484,7 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <v>1210229</v>
+        <v>2454926</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -495,7 +495,7 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <v>1187668</v>
+        <v>2401611</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -506,7 +506,7 @@
         <v>6</v>
       </c>
       <c r="C6">
-        <v>1079223</v>
+        <v>2145422</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -517,7 +517,7 @@
         <v>7</v>
       </c>
       <c r="C7">
-        <v>980015</v>
+        <v>1822575</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -528,7 +528,7 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>858942</v>
+        <v>1727244</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -539,7 +539,7 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>791552</v>
+        <v>1632111</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -550,7 +550,7 @@
         <v>10</v>
       </c>
       <c r="C10">
-        <v>738545</v>
+        <v>1596603</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -561,7 +561,7 @@
         <v>11</v>
       </c>
       <c r="C11">
-        <v>346209</v>
+        <v>715924</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -572,7 +572,7 @@
         <v>12</v>
       </c>
       <c r="C12">
-        <v>328979</v>
+        <v>664018</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -583,7 +583,7 @@
         <v>13</v>
       </c>
       <c r="C13">
-        <v>308882</v>
+        <v>654796</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -594,7 +594,7 @@
         <v>14</v>
       </c>
       <c r="C14">
-        <v>264762</v>
+        <v>634195</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -605,7 +605,7 @@
         <v>15</v>
       </c>
       <c r="C15">
-        <v>217806</v>
+        <v>577967</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -616,7 +616,7 @@
         <v>16</v>
       </c>
       <c r="C16">
-        <v>188641</v>
+        <v>511980</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -627,7 +627,7 @@
         <v>17</v>
       </c>
       <c r="C17">
-        <v>185133</v>
+        <v>440864</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -638,7 +638,7 @@
         <v>18</v>
       </c>
       <c r="C18">
-        <v>177167</v>
+        <v>295395</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -649,7 +649,7 @@
         <v>19</v>
       </c>
       <c r="C19">
-        <v>139344</v>
+        <v>245353</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -660,7 +660,7 @@
         <v>20</v>
       </c>
       <c r="C20">
-        <v>83827</v>
+        <v>200103</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -671,7 +671,7 @@
         <v>21</v>
       </c>
       <c r="C21">
-        <v>39226</v>
+        <v>102127</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -682,7 +682,7 @@
         <v>22</v>
       </c>
       <c r="C22">
-        <v>31462</v>
+        <v>50647</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[UPD] update README.md and webserver.py
</commit_message>
<xml_diff>
--- a/Report_excel.xlsx
+++ b/Report_excel.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="s + + heet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -19,7 +19,7 @@
     <t>Region</t>
   </si>
   <si>
-    <t>Total Case</t>
+    <t>Total Case to date 13/04/2023</t>
   </si>
   <si>
     <t>Lombardia</t>
@@ -462,7 +462,7 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>4140912</v>
+        <v>4143150</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -473,7 +473,7 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>2710818</v>
+        <v>2712436</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -484,7 +484,7 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <v>2454926</v>
+        <v>2456161</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -495,7 +495,7 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <v>2401611</v>
+        <v>2402802</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -506,7 +506,7 @@
         <v>6</v>
       </c>
       <c r="C6">
-        <v>2145422</v>
+        <v>2146082</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -517,7 +517,7 @@
         <v>7</v>
       </c>
       <c r="C7">
-        <v>1822575</v>
+        <v>1822963</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -528,7 +528,7 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>1727244</v>
+        <v>1728126</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -539,7 +539,7 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>1632111</v>
+        <v>1632702</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -550,7 +550,7 @@
         <v>10</v>
       </c>
       <c r="C10">
-        <v>1596603</v>
+        <v>1597294</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -561,7 +561,7 @@
         <v>11</v>
       </c>
       <c r="C11">
-        <v>715924</v>
+        <v>716098</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -572,7 +572,7 @@
         <v>12</v>
       </c>
       <c r="C12">
-        <v>664018</v>
+        <v>664258</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -583,7 +583,7 @@
         <v>13</v>
       </c>
       <c r="C13">
-        <v>654796</v>
+        <v>655155</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -594,7 +594,7 @@
         <v>14</v>
       </c>
       <c r="C14">
-        <v>634195</v>
+        <v>634472</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -605,7 +605,7 @@
         <v>15</v>
       </c>
       <c r="C15">
-        <v>577967</v>
+        <v>578199</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -616,7 +616,7 @@
         <v>16</v>
       </c>
       <c r="C16">
-        <v>511980</v>
+        <v>512209</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -627,7 +627,7 @@
         <v>17</v>
       </c>
       <c r="C17">
-        <v>440864</v>
+        <v>441114</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -638,7 +638,7 @@
         <v>18</v>
       </c>
       <c r="C18">
-        <v>295395</v>
+        <v>295517</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -649,7 +649,7 @@
         <v>19</v>
       </c>
       <c r="C19">
-        <v>245353</v>
+        <v>245446</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -660,7 +660,7 @@
         <v>20</v>
       </c>
       <c r="C20">
-        <v>200103</v>
+        <v>200156</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -671,7 +671,7 @@
         <v>21</v>
       </c>
       <c r="C21">
-        <v>102127</v>
+        <v>102165</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -682,7 +682,7 @@
         <v>22</v>
       </c>
       <c r="C22">
-        <v>50647</v>
+        <v>50665</v>
       </c>
     </row>
   </sheetData>

</xml_diff>